<commit_message>
RB bug fix  vignette update
</commit_message>
<xml_diff>
--- a/data/Env_Additonal_Sites.xlsx
+++ b/data/Env_Additonal_Sites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://apemltd365.sharepoint.com/sites/5874-HydroEcologyToolkit/Shared Documents/HE Toolkit/MASTER/hetoolkit/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rosalindb\Desktop\MASTER\hetoolkit_updated\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{82C208BE-6CA6-4A69-877F-FA37A822669A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{37E6F556-F6E7-4FFA-99E1-153D14882CF8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B05DB4-3069-4842-BFE9-B30DDF608C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C6D0E3BD-2704-4784-88F3-75F1FDC8D46D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>WATER_BODY</t>
   </si>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF5BF30-8159-4BB4-96D6-FA5A28B4515D}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,52 +693,52 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>34343</v>
+        <v>33597</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5">
-        <v>27886</v>
+        <v>24242</v>
       </c>
       <c r="E5">
-        <v>13403</v>
+        <v>15029</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
       </c>
       <c r="G5">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5">
-        <v>18.190000000000001</v>
+        <v>14</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="L5">
-        <v>26.33</v>
+        <v>30</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="N5">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="O5">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="P5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="Q5">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -746,52 +746,52 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>33597</v>
+        <v>33407</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6">
-        <v>24242</v>
+        <v>23090</v>
       </c>
       <c r="E6">
-        <v>15029</v>
+        <v>16100</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H6">
         <v>3</v>
       </c>
       <c r="I6">
-        <v>14</v>
+        <v>11.5</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6">
-        <v>4.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="L6">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="M6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="N6">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="O6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Q6">
-        <v>254</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -799,52 +799,52 @@
         <v>19</v>
       </c>
       <c r="B7">
-        <v>33407</v>
+        <v>33408</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
       </c>
       <c r="D7">
-        <v>23090</v>
+        <v>22669</v>
       </c>
       <c r="E7">
-        <v>16100</v>
+        <v>16930</v>
       </c>
       <c r="F7" t="s">
         <v>22</v>
       </c>
       <c r="G7">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H7">
         <v>3</v>
       </c>
       <c r="I7">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
       <c r="K7">
-        <v>4.4000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="L7">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="M7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N7">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="O7">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="P7">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q7">
-        <v>228</v>
+        <v>253.1</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -852,52 +852,52 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>33408</v>
+        <v>81318</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8">
-        <v>22669</v>
+        <v>21022</v>
       </c>
       <c r="E8">
-        <v>16930</v>
+        <v>17536</v>
       </c>
       <c r="F8" t="s">
         <v>22</v>
       </c>
       <c r="G8">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
       <c r="I8">
-        <v>10.5</v>
+        <v>8.9</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="L8">
         <v>30</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="O8">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="P8">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="Q8">
-        <v>253.1</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -905,28 +905,28 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>81318</v>
+        <v>34171</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
       <c r="D9">
-        <v>21022</v>
+        <v>20754</v>
       </c>
       <c r="E9">
-        <v>17536</v>
+        <v>18006</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="G9">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H9">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="I9">
-        <v>8.9</v>
+        <v>7.31</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -935,19 +935,19 @@
         <v>4.5</v>
       </c>
       <c r="L9">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="N9">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="O9">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="P9">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="Q9">
         <v>254</v>
@@ -958,104 +958,51 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>34171</v>
+        <v>33731</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
       <c r="D10">
-        <v>20754</v>
+        <v>18411</v>
       </c>
       <c r="E10">
-        <v>18006</v>
+        <v>21220</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="H10">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="I10">
-        <v>7.31</v>
+        <v>2.65</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="M10">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="N10">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="O10">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="P10">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="Q10">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
-        <v>33731</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11">
-        <v>18411</v>
-      </c>
-      <c r="E11">
-        <v>21220</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11">
-        <v>88</v>
-      </c>
-      <c r="H11">
-        <v>3.2</v>
-      </c>
-      <c r="I11">
-        <v>2.65</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>3</v>
-      </c>
-      <c r="L11">
-        <v>20</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>73</v>
-      </c>
-      <c r="O11">
-        <v>13</v>
-      </c>
-      <c r="P11">
-        <v>13</v>
-      </c>
-      <c r="Q11">
         <v>253.1</v>
       </c>
     </row>
@@ -1065,18 +1012,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1285,6 +1232,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{740B79D2-7F1E-4FBB-A102-3182606BD28B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E95C756A-9B50-485E-A360-A3970EBC2683}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1293,14 +1248,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{740B79D2-7F1E-4FBB-A102-3182606BD28B}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B859BD3E-1318-41E9-B700-82CF03B02490}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dcdc6d01-573a-4199-8236-6dd299a9003d"/>
+    <ds:schemaRef ds:uri="181f6511-b771-4ae5-8f70-5f3e197c3b74"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B859BD3E-1318-41E9-B700-82CF03B02490}"/>
 </file>
</xml_diff>